<commit_message>
bottleneck and tps details added
</commit_message>
<xml_diff>
--- a/resources/bottleneck-or-stresstest-point.xlsx
+++ b/resources/bottleneck-or-stresstest-point.xlsx
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F6:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>